<commit_message>
Version finale enregistrement excel
Lorsque l'arduino est déconnecté, un fichier excel se créer automatiquement avec les valeurs de RPM (dédoublé) a chaque seconde.
On ne peut pas utiliser le serialMonitor de arduino IDE en même temps que le programme python.
</commit_message>
<xml_diff>
--- a/Python/output.xlsx
+++ b/Python/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,63 @@
       <c r="N1" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -480,77 +537,191 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1
+          <t xml:space="preserve">Setup done
 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1
+          <t xml:space="preserve">0.00
 </t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0
-</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr"/>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.00
+</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Code réécrit et avec commentaire
Il reste la gestion de s'il n'y a pas de port de connecter à s'occuper
</commit_message>
<xml_diff>
--- a/Python/output.xlsx
+++ b/Python/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,66 +470,6 @@
       <c r="M1" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="1" t="n">
-        <v>31</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -591,7 +531,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.00
+          <t xml:space="preserve">0.88
 </t>
         </is>
       </c>
@@ -601,127 +541,7 @@
 </t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.00
-</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>